<commit_message>
Final Commit for Saturday
</commit_message>
<xml_diff>
--- a/DataSets/BotResults(Mine).xlsx
+++ b/DataSets/BotResults(Mine).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Dissertation_Artefact\DataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE954211-FFD9-42D0-A8A1-CF3E0A7913AD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1B9073-51C6-479C-AED5-FCE6B51C77F2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{54C24EBF-4E94-473C-9F52-99BEA4E6395E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$67:$T$140</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$67:$T$148</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$AA$25</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$AA$26:$AA$35</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$Z$1</definedName>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2842" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="938">
   <si>
     <t>Round/Game</t>
   </si>
@@ -2817,6 +2817,39 @@
   </si>
   <si>
     <t>Avg Game Length VS POSH</t>
+  </si>
+  <si>
+    <t>Round 1</t>
+  </si>
+  <si>
+    <t>Round 2</t>
+  </si>
+  <si>
+    <t>Round 3</t>
+  </si>
+  <si>
+    <t>Round 4</t>
+  </si>
+  <si>
+    <t>Round 5</t>
+  </si>
+  <si>
+    <t>Round 6</t>
+  </si>
+  <si>
+    <t>Round 7</t>
+  </si>
+  <si>
+    <t>Round 8</t>
+  </si>
+  <si>
+    <t>Matches Won</t>
+  </si>
+  <si>
+    <t>Avg POSH Score</t>
+  </si>
+  <si>
+    <t>Avg Oponent Score</t>
   </si>
 </sst>
 </file>
@@ -2983,7 +3016,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -3149,6 +3182,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -3159,13 +3201,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3416,6 +3478,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3425,43 +3490,93 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="45" fontId="0" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="45" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="45" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="8" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="45" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="45" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="45" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="21" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="45" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -18554,21 +18669,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF4D8A81-C279-40E8-A672-2309C37F83C5}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:CE186"/>
+  <dimension ref="A1:CE190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N186" sqref="C186:N186"/>
+    <sheetView tabSelected="1" topLeftCell="B146" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E157" sqref="E157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="11" style="59" customWidth="1"/>
-    <col min="3" max="3" width="12" style="59" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" customWidth="1"/>
@@ -18581,6 +18696,8 @@
     <col min="22" max="22" width="15" customWidth="1"/>
     <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.5703125" customWidth="1"/>
+    <col min="57" max="57" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18729,6 +18846,33 @@
       <c r="AD3" s="6">
         <v>0</v>
       </c>
+      <c r="AO3" s="146" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP3" s="147" t="s">
+        <v>927</v>
+      </c>
+      <c r="AQ3" s="147" t="s">
+        <v>928</v>
+      </c>
+      <c r="AR3" s="147" t="s">
+        <v>929</v>
+      </c>
+      <c r="AS3" s="147" t="s">
+        <v>930</v>
+      </c>
+      <c r="AT3" s="147" t="s">
+        <v>931</v>
+      </c>
+      <c r="AU3" s="147" t="s">
+        <v>932</v>
+      </c>
+      <c r="AV3" s="147" t="s">
+        <v>933</v>
+      </c>
+      <c r="AW3" s="147" t="s">
+        <v>934</v>
+      </c>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -18778,6 +18922,17 @@
       <c r="AD4" s="6">
         <v>0</v>
       </c>
+      <c r="AO4" s="148" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP4" s="149"/>
+      <c r="AQ4" s="149"/>
+      <c r="AR4" s="149"/>
+      <c r="AS4" s="149"/>
+      <c r="AT4" s="150"/>
+      <c r="AU4" s="149"/>
+      <c r="AV4" s="149"/>
+      <c r="AW4" s="149"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -18827,6 +18982,17 @@
       <c r="AD5" s="6">
         <v>2</v>
       </c>
+      <c r="AO5" s="151" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP5" s="152"/>
+      <c r="AQ5" s="152"/>
+      <c r="AR5" s="152"/>
+      <c r="AS5" s="152"/>
+      <c r="AT5" s="153"/>
+      <c r="AU5" s="152"/>
+      <c r="AV5" s="152"/>
+      <c r="AW5" s="152"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -18876,6 +19042,20 @@
       <c r="AD6" s="6">
         <v>7</v>
       </c>
+      <c r="AO6" s="151" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP6" s="149"/>
+      <c r="AQ6" s="149"/>
+      <c r="AR6" s="149"/>
+      <c r="AS6" s="149"/>
+      <c r="AT6" s="150"/>
+      <c r="AU6" s="149"/>
+      <c r="AV6" s="149"/>
+      <c r="AW6" s="149"/>
+      <c r="BE6" s="155">
+        <v>32647</v>
+      </c>
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -18925,6 +19105,20 @@
       <c r="AD7" s="6">
         <v>73</v>
       </c>
+      <c r="AO7" s="154" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP7" s="152"/>
+      <c r="AQ7" s="152"/>
+      <c r="AR7" s="152"/>
+      <c r="AS7" s="152"/>
+      <c r="AT7" s="153"/>
+      <c r="AU7" s="152"/>
+      <c r="AV7" s="152"/>
+      <c r="AW7" s="152"/>
+      <c r="BE7" s="156">
+        <v>11765</v>
+      </c>
     </row>
     <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -18974,7 +19168,17 @@
       <c r="AD8" s="6">
         <v>27</v>
       </c>
-      <c r="AW8" s="39"/>
+      <c r="AO8" s="154" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP8" s="149"/>
+      <c r="AQ8" s="149"/>
+      <c r="AR8" s="149"/>
+      <c r="AS8" s="149"/>
+      <c r="AT8" s="150"/>
+      <c r="AU8" s="149"/>
+      <c r="AV8" s="149"/>
+      <c r="AW8" s="149"/>
       <c r="AX8" s="40"/>
       <c r="AY8" s="40"/>
       <c r="AZ8" s="39"/>
@@ -18982,7 +19186,9 @@
       <c r="BB8" s="39"/>
       <c r="BC8" s="41"/>
       <c r="BD8" s="39"/>
-      <c r="BE8" s="39"/>
+      <c r="BE8" s="156">
+        <v>8932</v>
+      </c>
       <c r="BF8" s="39"/>
       <c r="BG8" s="39"/>
       <c r="BH8" s="39"/>
@@ -19041,7 +19247,17 @@
       <c r="AD9" s="6">
         <v>0</v>
       </c>
-      <c r="AW9" s="39"/>
+      <c r="AO9" s="151" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP9" s="152"/>
+      <c r="AQ9" s="152"/>
+      <c r="AR9" s="152"/>
+      <c r="AS9" s="152"/>
+      <c r="AT9" s="153"/>
+      <c r="AU9" s="152"/>
+      <c r="AV9" s="152"/>
+      <c r="AW9" s="152"/>
       <c r="AX9" s="40"/>
       <c r="AY9" s="40"/>
       <c r="AZ9" s="39"/>
@@ -19049,7 +19265,9 @@
       <c r="BB9" s="39"/>
       <c r="BC9" s="41"/>
       <c r="BD9" s="39"/>
-      <c r="BE9" s="39"/>
+      <c r="BE9" s="155">
+        <v>85071</v>
+      </c>
       <c r="BF9" s="39"/>
       <c r="BG9" s="39"/>
       <c r="BH9" s="39"/>
@@ -19108,7 +19326,19 @@
       <c r="AD10" s="6">
         <v>128</v>
       </c>
-      <c r="AW10" s="39"/>
+      <c r="AO10" s="148" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP10" s="149">
+        <v>52745</v>
+      </c>
+      <c r="AQ10" s="149"/>
+      <c r="AR10" s="149"/>
+      <c r="AS10" s="149"/>
+      <c r="AT10" s="150"/>
+      <c r="AU10" s="149"/>
+      <c r="AV10" s="149"/>
+      <c r="AW10" s="149"/>
       <c r="AX10" s="40"/>
       <c r="AY10" s="40"/>
       <c r="AZ10" s="39"/>
@@ -19116,7 +19346,9 @@
       <c r="BB10" s="39"/>
       <c r="BC10" s="41"/>
       <c r="BD10" s="39"/>
-      <c r="BE10" s="39"/>
+      <c r="BE10" s="155">
+        <v>19890</v>
+      </c>
       <c r="BF10" s="39"/>
       <c r="BG10" s="39"/>
       <c r="BH10" s="39"/>
@@ -19175,7 +19407,19 @@
       <c r="AD11" s="6">
         <v>2</v>
       </c>
-      <c r="AW11" s="39"/>
+      <c r="AO11" s="154" t="s">
+        <v>25</v>
+      </c>
+      <c r="AP11" s="152">
+        <v>23027</v>
+      </c>
+      <c r="AQ11" s="152"/>
+      <c r="AR11" s="152"/>
+      <c r="AS11" s="152"/>
+      <c r="AT11" s="153"/>
+      <c r="AU11" s="152"/>
+      <c r="AV11" s="152"/>
+      <c r="AW11" s="152"/>
       <c r="AX11" s="40"/>
       <c r="AY11" s="40"/>
       <c r="AZ11" s="39"/>
@@ -19183,7 +19427,9 @@
       <c r="BB11" s="39"/>
       <c r="BC11" s="41"/>
       <c r="BD11" s="39"/>
-      <c r="BE11" s="39"/>
+      <c r="BE11" s="156">
+        <v>7200</v>
+      </c>
       <c r="BF11" s="39"/>
       <c r="BG11" s="39"/>
       <c r="BH11" s="39"/>
@@ -19242,7 +19488,17 @@
       <c r="AD12" s="6">
         <v>77</v>
       </c>
-      <c r="AW12" s="39"/>
+      <c r="AO12" s="151" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP12" s="149"/>
+      <c r="AQ12" s="149"/>
+      <c r="AR12" s="149"/>
+      <c r="AS12" s="149"/>
+      <c r="AT12" s="150"/>
+      <c r="AU12" s="149"/>
+      <c r="AV12" s="149"/>
+      <c r="AW12" s="149"/>
       <c r="AX12" s="40"/>
       <c r="AY12" s="40"/>
       <c r="AZ12" s="39"/>
@@ -19250,7 +19506,9 @@
       <c r="BB12" s="39"/>
       <c r="BC12" s="41"/>
       <c r="BD12" s="39"/>
-      <c r="BE12" s="39"/>
+      <c r="BE12" s="155">
+        <v>28429</v>
+      </c>
       <c r="BF12" s="39"/>
       <c r="BG12" s="39"/>
       <c r="BH12" s="39"/>
@@ -19309,7 +19567,17 @@
       <c r="AD13" s="6">
         <v>0</v>
       </c>
-      <c r="AW13" s="39"/>
+      <c r="AO13" s="154" t="s">
+        <v>148</v>
+      </c>
+      <c r="AP13" s="152"/>
+      <c r="AQ13" s="152"/>
+      <c r="AR13" s="152"/>
+      <c r="AS13" s="152"/>
+      <c r="AT13" s="153"/>
+      <c r="AU13" s="152"/>
+      <c r="AV13" s="152"/>
+      <c r="AW13" s="152"/>
       <c r="AX13" s="40"/>
       <c r="AY13" s="40"/>
       <c r="AZ13" s="39"/>
@@ -19317,7 +19585,9 @@
       <c r="BB13" s="39"/>
       <c r="BC13" s="41"/>
       <c r="BD13" s="39"/>
-      <c r="BE13" s="39"/>
+      <c r="BE13" s="156">
+        <v>10933</v>
+      </c>
       <c r="BF13" s="39"/>
       <c r="BG13" s="39"/>
       <c r="BH13" s="39"/>
@@ -19384,7 +19654,9 @@
       <c r="BB14" s="39"/>
       <c r="BC14" s="41"/>
       <c r="BD14" s="39"/>
-      <c r="BE14" s="39"/>
+      <c r="BE14" s="156">
+        <v>2377</v>
+      </c>
       <c r="BF14" s="39"/>
       <c r="BG14" s="39"/>
       <c r="BH14" s="39"/>
@@ -19585,7 +19857,10 @@
       <c r="BB17" s="39"/>
       <c r="BC17" s="41"/>
       <c r="BD17" s="39"/>
-      <c r="BE17" s="39"/>
+      <c r="BE17" s="157">
+        <f>SUM(BE6:BE14)/9</f>
+        <v>23027.111111111109</v>
+      </c>
       <c r="BF17" s="39"/>
       <c r="BG17" s="39"/>
       <c r="BH17" s="39"/>
@@ -22414,35 +22689,35 @@
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
       <c r="T58" s="43">
-        <f>SUM(I68:I140, I142:I149)/80</f>
+        <f>SUM(I68:I140, I141:I148)/80</f>
         <v>19551.674999999999</v>
       </c>
       <c r="U58" s="20">
-        <f>SUM(H68:H140,H142:H149)/80</f>
+        <f>SUM(H68:H140,H141:H148)/80</f>
         <v>26765.674999999999</v>
       </c>
       <c r="W58" s="20">
-        <f>SUM(I74,I80,I81,I88,I89,I96,I97,I104,I105,I113,I114,I122,I123,I131,I132,I139,I140,I143)/17</f>
+        <f>SUM(I74,I80,I81,I88,I89,I96,I97,I104,I105,I113,I114,I122,I123,I131,I132,I139,I140,I142)/17</f>
         <v>29369.529411764706</v>
       </c>
       <c r="X58" s="20">
-        <f>SUM(I71,I72,I73,I77,I78,I79,I85,I86,I87,I93,I94,I95,I101,I102,I103,I109,I110,I111,I112,I118,I119,I120,I121,I127,I128,I129,I130,I136,I137,I138,I142,I145,I146,I147,I148,I149)/36</f>
+        <f>SUM(I71,I72,I73,I77,I78,I79,I85,I86,I87,I93,I94,I95,I101,I102,I103,I109,I110,I111,I112,I118,I119,I120,I121,I127,I128,I129,I130,I136,I137,I138,I141,I144,I145,I146,I147,I148)/36</f>
         <v>24069.583333333332</v>
       </c>
       <c r="Y58" s="20">
-        <f>SUM(I68,I69,I70,I75,I76,I82,I83,I84,I90,I91,I92,I98,I99,I100,I106,I107,I108,I115,I116,I117,I124,I125,I126,I133,I134,I135,I144)/27</f>
+        <f>SUM(I68,I69,I70,I75,I76,I82,I83,I84,I90,I91,I92,I98,I99,I100,I106,I107,I108,I115,I116,I117,I124,I125,I126,I133,I134,I135,I143)/27</f>
         <v>7346.1851851851852</v>
       </c>
       <c r="Z58" s="20">
-        <f>SUM(H74,H80,H81,H88,H89,H96,H97,H104,H105,H113,H114,H122,H123,H131,H132,H139,H140,H143)/17</f>
+        <f>SUM(H74,H80,H81,H88,H89,H96,H97,H104,H105,H113,H114,H122,H123,H131,H132,H139,H140,H142)/17</f>
         <v>33517.76470588235</v>
       </c>
       <c r="AA58" s="20">
-        <f>SUM(H71,H72,H73,H77,H78,H79,H85,H86,H93,H87,H94,H95,H101,H102,H103,H109,H110,H111,H112,H118,H119,H120,H121,H127,H128,H129,H130,H136,H137,H138,H142,H145,H146,H147,H148,H149)/36</f>
+        <f>SUM(H71,H72,H73,H77,H78,H79,H85,H86,H93,H87,H94,H95,H101,H102,H103,H109,H110,H111,H112,H118,H119,H120,H121,H127,H128,H129,H130,H136,H137,H138,H141,H144,H145,H146,H147,H148)/36</f>
         <v>26275.777777777777</v>
       </c>
       <c r="AB58" s="20">
-        <f>SUM(H68,H69,H70,H75,H76,H82,H83,H84,H90,H91,H92,H98,H99,H100,H106,H107,H108,H115,H117,H116,H124,H125,H126,H133,H135,H134,H144)/27</f>
+        <f>SUM(H68,H69,H70,H75,H76,H82,H83,H84,H90,H91,H92,H98,H99,H100,H106,H107,H108,H115,H117,H116,H124,H125,H126,H133,H135,H134,H143)/27</f>
         <v>23167.555555555555</v>
       </c>
       <c r="AW58" s="2"/>
@@ -22544,35 +22819,35 @@
         <v>368</v>
       </c>
       <c r="T60" s="43">
-        <f>_xlfn.STDEV.S(I68:I140, I142:I149)</f>
+        <f>_xlfn.STDEV.S(I68:I140, I141:I148)</f>
         <v>27391.800735094272</v>
       </c>
       <c r="U60" s="43">
-        <f>_xlfn.STDEV.P(H68:H140,H142:H149)</f>
+        <f>_xlfn.STDEV.P(H68:H140,H141:H148)</f>
         <v>18616.993045497144</v>
       </c>
       <c r="W60" s="20">
-        <f>_xlfn.STDEV.P(I74,I80,I81,I88,I89,I96,I97,I104,I105,I113,I114,I122,I123,I131,I132,I139,I140,I143)</f>
+        <f>_xlfn.STDEV.P(I74,I80,I81,I88,I89,I96,I97,I104,I105,I113,I114,I122,I123,I131,I132,I139,I140,I142)</f>
         <v>17778.12334455808</v>
       </c>
       <c r="X60" s="20">
-        <f>_xlfn.STDEV.P(I71,I72,I73,I77,I78,I79,I85,I86,I87,I93,I94,I95,I101,I102,I103,I109,I110,I111,I112,I118,I119,I120,I121,I127,I128,I129,I130,I136,I137,I138,I142,I145,I146,I147,I148,I149)</f>
+        <f>_xlfn.STDEV.P(I71,I72,I73,I77,I78,I79,I85,I86,I87,I93,I94,I95,I101,I102,I103,I109,I110,I111,I112,I118,I119,I120,I121,I127,I128,I129,I130,I136,I137,I138,I141,I144,I145,I146,I147,I148)</f>
         <v>36435.94911803375</v>
       </c>
       <c r="Y60" s="20">
-        <f>_xlfn.STDEV.P(I68,I69,I70,I75,I76,I82,I83,I84,I90,I91,I92,I98,I99,I100,I106,I107,I108,I115,I116,I117,I124,I125,I126,I133,I134,I135,I144)</f>
+        <f>_xlfn.STDEV.P(I68,I69,I70,I75,I76,I82,I83,I84,I90,I91,I92,I98,I99,I100,I106,I107,I108,I115,I116,I117,I124,I125,I126,I133,I134,I135,I143)</f>
         <v>4651.8893894451503</v>
       </c>
       <c r="Z60" s="20">
-        <f>_xlfn.STDEV.P(H74,H80,H81,H88,H89,H96,H97,H104,H105,H113,H114,H122,H123,H131,H132,H139,H140,H143)</f>
+        <f>_xlfn.STDEV.P(H74,H80,H81,H88,H89,H96,H97,H104,H105,H113,H114,H122,H123,H131,H132,H139,H140,H142)</f>
         <v>19071.083287998554</v>
       </c>
       <c r="AA60" s="20">
-        <f>_xlfn.STDEV.P(H71,H72,H73,H77,H78,H79,H85,H86,H93,H87,H94,H95,H101,H102,H103,H109,H110,H111,H112,H118,H119,H120,H121,H127,H128,H129,H130,H136,H137,H138,H142,H145,H146,H147,H148,H149)</f>
+        <f>_xlfn.STDEV.P(H71,H72,H73,H77,H78,H79,H85,H86,H93,H87,H94,H95,H101,H102,H103,H109,H110,H111,H112,H118,H119,H120,H121,H127,H128,H129,H130,H136,H137,H138,H141,H144,H145,H146,H147,H148)</f>
         <v>19881.254247421548</v>
       </c>
       <c r="AB60" s="20">
-        <f>_xlfn.STDEV.P(H68,H69,H70,H75,H76,H82,H83,H84,H90,H91,H92,H98,H99,H100,H106,H107,H108,H115,H117,H116,H124,H125,H126,H133,H135,H134,H144)</f>
+        <f>_xlfn.STDEV.P(H68,H69,H70,H75,H76,H82,H83,H84,H90,H91,H92,H98,H99,H100,H106,H107,H108,H115,H117,H116,H124,H125,H126,H133,H135,H134,H143)</f>
         <v>15537.28468658854</v>
       </c>
       <c r="AW60" s="2"/>
@@ -24009,7 +24284,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="72" spans="1:83" ht="21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:83" ht="21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
         <v>30</v>
       </c>
@@ -25366,7 +25641,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="78" spans="1:83" ht="21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:83" ht="21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
         <v>82</v>
       </c>
@@ -27176,7 +27451,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="86" spans="1:83" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:83" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
         <v>100</v>
       </c>
@@ -28986,7 +29261,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="94" spans="1:83" ht="21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:83" ht="21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="30" t="s">
         <v>113</v>
       </c>
@@ -30798,7 +31073,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="102" spans="1:83" ht="21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:83" ht="21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="30" t="s">
         <v>242</v>
       </c>
@@ -32610,7 +32885,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="110" spans="1:83" ht="21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:83" ht="21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="30" t="s">
         <v>266</v>
       </c>
@@ -34648,7 +34923,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="119" spans="1:83" ht="21" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:83" ht="21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="33" t="s">
         <v>293</v>
       </c>
@@ -36684,7 +36959,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="128" spans="1:83" ht="21" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:83" ht="21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="30" t="s">
         <v>321</v>
       </c>
@@ -38720,7 +38995,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="137" spans="1:83" ht="21" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:83" ht="21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="33" t="s">
         <v>348</v>
       </c>
@@ -39625,6 +39900,62 @@
       </c>
     </row>
     <row r="141" spans="1:83" ht="21" x14ac:dyDescent="0.25">
+      <c r="A141" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B141" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C141" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="D141" s="30"/>
+      <c r="E141" s="30"/>
+      <c r="F141" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G141" s="81">
+        <v>4.1331018518518517E-2</v>
+      </c>
+      <c r="H141" s="30">
+        <v>16095</v>
+      </c>
+      <c r="I141" s="30">
+        <v>66936</v>
+      </c>
+      <c r="J141" s="30">
+        <v>0.75953999999999999</v>
+      </c>
+      <c r="K141" s="30">
+        <v>0</v>
+      </c>
+      <c r="L141" s="30">
+        <v>0</v>
+      </c>
+      <c r="M141" s="30">
+        <v>0</v>
+      </c>
+      <c r="N141" s="30">
+        <v>0</v>
+      </c>
+      <c r="O141" s="30">
+        <v>0</v>
+      </c>
+      <c r="P141" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q141" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="R141" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="S141" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="T141" s="30" t="s">
+        <v>153</v>
+      </c>
       <c r="V141" s="33" t="s">
         <v>570</v>
       </c>
@@ -39795,61 +40126,61 @@
       </c>
     </row>
     <row r="142" spans="1:83" ht="21" x14ac:dyDescent="0.25">
-      <c r="A142" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B142" s="56" t="s">
+      <c r="A142" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B142" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="C142" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="D142" s="30"/>
-      <c r="E142" s="30"/>
-      <c r="F142" s="30" t="s">
+      <c r="C142" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="D142" s="33"/>
+      <c r="E142" s="33"/>
+      <c r="F142" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="G142" s="81">
-        <v>4.1331018518518517E-2</v>
-      </c>
-      <c r="H142" s="30">
-        <v>16095</v>
-      </c>
-      <c r="I142" s="30">
-        <v>66936</v>
-      </c>
-      <c r="J142" s="30">
-        <v>0.75953999999999999</v>
-      </c>
-      <c r="K142" s="30">
-        <v>0</v>
-      </c>
-      <c r="L142" s="30">
-        <v>0</v>
-      </c>
-      <c r="M142" s="30">
-        <v>0</v>
-      </c>
-      <c r="N142" s="30">
-        <v>0</v>
-      </c>
-      <c r="O142" s="30">
-        <v>0</v>
-      </c>
-      <c r="P142" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q142" s="30" t="s">
+      <c r="G142" s="82">
+        <v>1.59375E-2</v>
+      </c>
+      <c r="H142" s="33">
+        <v>34845</v>
+      </c>
+      <c r="I142" s="33">
+        <v>54879</v>
+      </c>
+      <c r="J142" s="33">
+        <v>0.36504999999999999</v>
+      </c>
+      <c r="K142" s="33">
+        <v>0</v>
+      </c>
+      <c r="L142" s="33">
+        <v>0</v>
+      </c>
+      <c r="M142" s="33">
+        <v>0</v>
+      </c>
+      <c r="N142" s="33">
+        <v>0</v>
+      </c>
+      <c r="O142" s="33">
+        <v>0</v>
+      </c>
+      <c r="P142" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q142" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="R142" s="30" t="s">
+      <c r="R142" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="S142" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="T142" s="30" t="s">
-        <v>153</v>
+      <c r="S142" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="T142" s="33" t="s">
+        <v>155</v>
       </c>
       <c r="V142" s="30" t="s">
         <v>573</v>
@@ -40021,61 +40352,63 @@
       </c>
     </row>
     <row r="143" spans="1:83" ht="21" x14ac:dyDescent="0.25">
-      <c r="A143" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B143" s="57" t="s">
+      <c r="A143" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B143" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="C143" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="D143" s="33"/>
-      <c r="E143" s="33"/>
-      <c r="F143" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G143" s="82">
-        <v>1.59375E-2</v>
-      </c>
-      <c r="H143" s="33">
-        <v>34845</v>
-      </c>
-      <c r="I143" s="33">
-        <v>54879</v>
-      </c>
-      <c r="J143" s="33">
-        <v>0.36504999999999999</v>
-      </c>
-      <c r="K143" s="33">
-        <v>0</v>
-      </c>
-      <c r="L143" s="33">
-        <v>0</v>
-      </c>
-      <c r="M143" s="33">
-        <v>0</v>
-      </c>
-      <c r="N143" s="33">
-        <v>0</v>
-      </c>
-      <c r="O143" s="33">
-        <v>0</v>
-      </c>
-      <c r="P143" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q143" s="33" t="s">
+      <c r="C143" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="D143" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E143" s="30"/>
+      <c r="F143" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G143" s="81">
+        <v>4.6990740740740743E-3</v>
+      </c>
+      <c r="H143" s="30">
+        <v>10342</v>
+      </c>
+      <c r="I143" s="30">
+        <v>4117</v>
+      </c>
+      <c r="J143" s="30">
+        <v>-0.60185999999999995</v>
+      </c>
+      <c r="K143" s="30">
+        <v>0</v>
+      </c>
+      <c r="L143" s="30">
+        <v>0</v>
+      </c>
+      <c r="M143" s="30">
+        <v>0</v>
+      </c>
+      <c r="N143" s="30">
+        <v>1</v>
+      </c>
+      <c r="O143" s="30">
+        <v>0</v>
+      </c>
+      <c r="P143" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q143" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="R143" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="R143" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="S143" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="T143" s="33" t="s">
-        <v>155</v>
+      <c r="S143" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="T143" s="30" t="s">
+        <v>157</v>
       </c>
       <c r="V143" s="33" t="s">
         <v>576</v>
@@ -40247,63 +40580,61 @@
       </c>
     </row>
     <row r="144" spans="1:83" ht="21" x14ac:dyDescent="0.25">
-      <c r="A144" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B144" s="56" t="s">
+      <c r="A144" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B144" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="C144" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="D144" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E144" s="30"/>
-      <c r="F144" s="30" t="s">
+      <c r="C144" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="D144" s="33"/>
+      <c r="E144" s="33"/>
+      <c r="F144" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="G144" s="81">
-        <v>4.6990740740740743E-3</v>
-      </c>
-      <c r="H144" s="30">
-        <v>10342</v>
-      </c>
-      <c r="I144" s="30">
-        <v>4117</v>
-      </c>
-      <c r="J144" s="30">
-        <v>-0.60185999999999995</v>
-      </c>
-      <c r="K144" s="30">
-        <v>0</v>
-      </c>
-      <c r="L144" s="30">
-        <v>0</v>
-      </c>
-      <c r="M144" s="30">
-        <v>0</v>
-      </c>
-      <c r="N144" s="30">
-        <v>1</v>
-      </c>
-      <c r="O144" s="30">
-        <v>0</v>
-      </c>
-      <c r="P144" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q144" s="30" t="s">
+      <c r="G144" s="82">
+        <v>4.1331018518518517E-2</v>
+      </c>
+      <c r="H144" s="33">
+        <v>68081</v>
+      </c>
+      <c r="I144" s="33">
+        <v>146057</v>
+      </c>
+      <c r="J144" s="33">
+        <v>0.53386999999999996</v>
+      </c>
+      <c r="K144" s="33">
+        <v>0</v>
+      </c>
+      <c r="L144" s="33">
+        <v>0</v>
+      </c>
+      <c r="M144" s="33">
+        <v>0</v>
+      </c>
+      <c r="N144" s="33">
+        <v>0</v>
+      </c>
+      <c r="O144" s="33">
+        <v>0</v>
+      </c>
+      <c r="P144" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q144" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="R144" s="30" t="s">
+      <c r="R144" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="S144" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="T144" s="30" t="s">
-        <v>157</v>
+      <c r="S144" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="T144" s="33" t="s">
+        <v>159</v>
       </c>
       <c r="V144" s="30" t="s">
         <v>579</v>
@@ -40475,61 +40806,61 @@
       </c>
     </row>
     <row r="145" spans="1:83" ht="21" x14ac:dyDescent="0.25">
-      <c r="A145" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="B145" s="57" t="s">
+      <c r="A145" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B145" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="C145" s="57" t="s">
+      <c r="C145" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="D145" s="33"/>
-      <c r="E145" s="33"/>
-      <c r="F145" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G145" s="82">
+      <c r="D145" s="30"/>
+      <c r="E145" s="30"/>
+      <c r="F145" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G145" s="81">
         <v>4.1331018518518517E-2</v>
       </c>
-      <c r="H145" s="33">
-        <v>68081</v>
-      </c>
-      <c r="I145" s="33">
-        <v>146057</v>
-      </c>
-      <c r="J145" s="33">
-        <v>0.53386999999999996</v>
-      </c>
-      <c r="K145" s="33">
-        <v>0</v>
-      </c>
-      <c r="L145" s="33">
-        <v>0</v>
-      </c>
-      <c r="M145" s="33">
-        <v>0</v>
-      </c>
-      <c r="N145" s="33">
-        <v>0</v>
-      </c>
-      <c r="O145" s="33">
-        <v>0</v>
-      </c>
-      <c r="P145" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q145" s="33" t="s">
+      <c r="H145" s="30">
+        <v>30350</v>
+      </c>
+      <c r="I145" s="30">
+        <v>73503</v>
+      </c>
+      <c r="J145" s="30">
+        <v>0.58708000000000005</v>
+      </c>
+      <c r="K145" s="30">
+        <v>0</v>
+      </c>
+      <c r="L145" s="30">
+        <v>0</v>
+      </c>
+      <c r="M145" s="30">
+        <v>0</v>
+      </c>
+      <c r="N145" s="30">
+        <v>0</v>
+      </c>
+      <c r="O145" s="30">
+        <v>0</v>
+      </c>
+      <c r="P145" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q145" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="R145" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="R145" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="S145" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="T145" s="33" t="s">
-        <v>159</v>
+      <c r="S145" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="T145" s="30" t="s">
+        <v>161</v>
       </c>
       <c r="V145" s="33" t="s">
         <v>582</v>
@@ -40701,61 +41032,61 @@
       </c>
     </row>
     <row r="146" spans="1:83" ht="21" x14ac:dyDescent="0.25">
-      <c r="A146" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B146" s="56" t="s">
+      <c r="A146" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B146" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="C146" s="56" t="s">
+      <c r="C146" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D146" s="30"/>
-      <c r="E146" s="30"/>
-      <c r="F146" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="G146" s="81">
-        <v>4.1331018518518517E-2</v>
-      </c>
-      <c r="H146" s="30">
-        <v>30350</v>
-      </c>
-      <c r="I146" s="30">
-        <v>73503</v>
-      </c>
-      <c r="J146" s="30">
-        <v>0.58708000000000005</v>
-      </c>
-      <c r="K146" s="30">
-        <v>0</v>
-      </c>
-      <c r="L146" s="30">
-        <v>0</v>
-      </c>
-      <c r="M146" s="30">
-        <v>0</v>
-      </c>
-      <c r="N146" s="30">
-        <v>0</v>
-      </c>
-      <c r="O146" s="30">
-        <v>0</v>
-      </c>
-      <c r="P146" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q146" s="30" t="s">
+      <c r="D146" s="33"/>
+      <c r="E146" s="33"/>
+      <c r="F146" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G146" s="82">
+        <v>7.6504629629629631E-3</v>
+      </c>
+      <c r="H146" s="33">
+        <v>8108</v>
+      </c>
+      <c r="I146" s="33">
+        <v>13701</v>
+      </c>
+      <c r="J146" s="33">
+        <v>0.40819</v>
+      </c>
+      <c r="K146" s="33">
+        <v>0</v>
+      </c>
+      <c r="L146" s="33">
+        <v>0</v>
+      </c>
+      <c r="M146" s="33">
+        <v>0</v>
+      </c>
+      <c r="N146" s="33">
+        <v>0</v>
+      </c>
+      <c r="O146" s="33">
+        <v>0</v>
+      </c>
+      <c r="P146" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q146" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="R146" s="30" t="s">
+      <c r="R146" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="S146" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="T146" s="30" t="s">
-        <v>161</v>
+      <c r="S146" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="T146" s="33" t="s">
+        <v>163</v>
       </c>
       <c r="V146" s="30" t="s">
         <v>585</v>
@@ -40927,61 +41258,61 @@
       </c>
     </row>
     <row r="147" spans="1:83" ht="21" x14ac:dyDescent="0.25">
-      <c r="A147" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="B147" s="57" t="s">
+      <c r="A147" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B147" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="C147" s="57" t="s">
+      <c r="C147" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="D147" s="33"/>
-      <c r="E147" s="33"/>
-      <c r="F147" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G147" s="82">
-        <v>7.6504629629629631E-3</v>
-      </c>
-      <c r="H147" s="33">
-        <v>8108</v>
-      </c>
-      <c r="I147" s="33">
-        <v>13701</v>
-      </c>
-      <c r="J147" s="33">
-        <v>0.40819</v>
-      </c>
-      <c r="K147" s="33">
-        <v>0</v>
-      </c>
-      <c r="L147" s="33">
-        <v>0</v>
-      </c>
-      <c r="M147" s="33">
-        <v>0</v>
-      </c>
-      <c r="N147" s="33">
-        <v>0</v>
-      </c>
-      <c r="O147" s="33">
-        <v>0</v>
-      </c>
-      <c r="P147" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q147" s="33" t="s">
+      <c r="D147" s="30"/>
+      <c r="E147" s="30"/>
+      <c r="F147" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G147" s="81">
+        <v>4.1331018518518517E-2</v>
+      </c>
+      <c r="H147" s="30">
+        <v>34480</v>
+      </c>
+      <c r="I147" s="30">
+        <v>78965</v>
+      </c>
+      <c r="J147" s="30">
+        <v>0.56333999999999995</v>
+      </c>
+      <c r="K147" s="30">
+        <v>0</v>
+      </c>
+      <c r="L147" s="30">
+        <v>0</v>
+      </c>
+      <c r="M147" s="30">
+        <v>0</v>
+      </c>
+      <c r="N147" s="30">
+        <v>0</v>
+      </c>
+      <c r="O147" s="30">
+        <v>0</v>
+      </c>
+      <c r="P147" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q147" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="R147" s="33" t="s">
+      <c r="R147" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="S147" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="T147" s="33" t="s">
-        <v>163</v>
+      <c r="S147" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="T147" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="V147" s="33" t="s">
         <v>588</v>
@@ -41153,61 +41484,61 @@
       </c>
     </row>
     <row r="148" spans="1:83" ht="21" x14ac:dyDescent="0.25">
-      <c r="A148" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="B148" s="56" t="s">
+      <c r="A148" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B148" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="C148" s="56" t="s">
+      <c r="C148" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D148" s="30"/>
-      <c r="E148" s="30"/>
-      <c r="F148" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="G148" s="81">
+      <c r="D148" s="33"/>
+      <c r="E148" s="33"/>
+      <c r="F148" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G148" s="82">
         <v>4.1331018518518517E-2</v>
       </c>
-      <c r="H148" s="30">
-        <v>34480</v>
-      </c>
-      <c r="I148" s="30">
-        <v>78965</v>
-      </c>
-      <c r="J148" s="30">
-        <v>0.56333999999999995</v>
-      </c>
-      <c r="K148" s="30">
-        <v>0</v>
-      </c>
-      <c r="L148" s="30">
-        <v>0</v>
-      </c>
-      <c r="M148" s="30">
-        <v>0</v>
-      </c>
-      <c r="N148" s="30">
-        <v>0</v>
-      </c>
-      <c r="O148" s="30">
-        <v>0</v>
-      </c>
-      <c r="P148" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q148" s="30" t="s">
+      <c r="H148" s="33">
+        <v>35594</v>
+      </c>
+      <c r="I148" s="33">
+        <v>91620</v>
+      </c>
+      <c r="J148" s="33">
+        <v>0.61150000000000004</v>
+      </c>
+      <c r="K148" s="33">
+        <v>0</v>
+      </c>
+      <c r="L148" s="33">
+        <v>0</v>
+      </c>
+      <c r="M148" s="33">
+        <v>0</v>
+      </c>
+      <c r="N148" s="33">
+        <v>0</v>
+      </c>
+      <c r="O148" s="33">
+        <v>0</v>
+      </c>
+      <c r="P148" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q148" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="R148" s="30" t="s">
+      <c r="R148" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="S148" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="T148" s="30" t="s">
-        <v>166</v>
+      <c r="S148" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="T148" s="33" t="s">
+        <v>169</v>
       </c>
       <c r="V148" s="30" t="s">
         <v>591</v>
@@ -41376,64 +41707,6 @@
       </c>
       <c r="CE148" s="30" t="s">
         <v>578</v>
-      </c>
-    </row>
-    <row r="149" spans="1:83" ht="21" x14ac:dyDescent="0.25">
-      <c r="A149" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="B149" s="57" t="s">
-        <v>148</v>
-      </c>
-      <c r="C149" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D149" s="33"/>
-      <c r="E149" s="33"/>
-      <c r="F149" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="G149" s="82">
-        <v>4.1331018518518517E-2</v>
-      </c>
-      <c r="H149" s="33">
-        <v>35594</v>
-      </c>
-      <c r="I149" s="33">
-        <v>91620</v>
-      </c>
-      <c r="J149" s="33">
-        <v>0.61150000000000004</v>
-      </c>
-      <c r="K149" s="33">
-        <v>0</v>
-      </c>
-      <c r="L149" s="33">
-        <v>0</v>
-      </c>
-      <c r="M149" s="33">
-        <v>0</v>
-      </c>
-      <c r="N149" s="33">
-        <v>0</v>
-      </c>
-      <c r="O149" s="33">
-        <v>0</v>
-      </c>
-      <c r="P149" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q149" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="R149" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="S149" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="T149" s="33" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="152" spans="1:83" x14ac:dyDescent="0.25">
@@ -41457,16 +41730,27 @@
       <c r="S152" s="39"/>
       <c r="T152" s="39"/>
     </row>
-    <row r="153" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="39"/>
       <c r="B153" s="46"/>
-      <c r="C153" s="46"/>
-      <c r="D153" s="39"/>
-      <c r="E153" s="39"/>
-      <c r="F153" s="39"/>
-      <c r="G153" s="41"/>
-      <c r="I153" s="39"/>
-      <c r="J153" s="39"/>
+      <c r="C153" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D153" s="80" t="s">
+        <v>935</v>
+      </c>
+      <c r="E153" s="80" t="s">
+        <v>379</v>
+      </c>
+      <c r="F153" s="80" t="s">
+        <v>936</v>
+      </c>
+      <c r="G153" s="160" t="s">
+        <v>937</v>
+      </c>
+      <c r="H153" s="159"/>
+      <c r="I153" s="158"/>
+      <c r="J153" s="158"/>
       <c r="K153" s="39"/>
       <c r="L153" s="39"/>
       <c r="M153" s="39"/>
@@ -41481,13 +41765,27 @@
     <row r="154" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A154" s="39"/>
       <c r="B154" s="46"/>
-      <c r="C154" s="46"/>
-      <c r="D154" s="39"/>
-      <c r="E154" s="39"/>
-      <c r="F154" s="39"/>
-      <c r="G154" s="41"/>
-      <c r="I154" s="39"/>
-      <c r="J154" s="39"/>
+      <c r="C154" s="64" t="s">
+        <v>381</v>
+      </c>
+      <c r="D154" s="80">
+        <v>8</v>
+      </c>
+      <c r="E154" s="161">
+        <f>SUM(G141,G142,G143,G145,G144,G146,G147,G148)/10</f>
+        <v>2.3494212962962956E-2</v>
+      </c>
+      <c r="F154" s="162">
+        <f>SUM(I141,I142,I143,I144,I145,I146,I147,I148)/10</f>
+        <v>52977.8</v>
+      </c>
+      <c r="G154" s="162">
+        <f>SUM(H141,H142,H143,H144,H145,H146,H147,H148)/10</f>
+        <v>23789.5</v>
+      </c>
+      <c r="H154" s="159"/>
+      <c r="I154" s="158"/>
+      <c r="J154" s="158"/>
       <c r="K154" s="39"/>
       <c r="L154" s="39"/>
       <c r="M154" s="39"/>
@@ -41506,7 +41804,6 @@
       <c r="D155" s="39"/>
       <c r="E155" s="39"/>
       <c r="F155" s="39"/>
-      <c r="G155" s="41"/>
       <c r="I155" s="39"/>
       <c r="J155" s="39"/>
       <c r="K155" s="39"/>
@@ -41800,7 +42097,7 @@
       </c>
       <c r="I165" s="48"/>
       <c r="K165" s="48"/>
-      <c r="L165" s="109">
+      <c r="L165" s="112">
         <f>SUM(I183-I186)/I183*100</f>
         <v>100</v>
       </c>
@@ -41821,19 +42118,19 @@
       <c r="C166" s="46"/>
       <c r="D166" s="39"/>
       <c r="E166" s="83">
-        <f>SUM(G68:G149)/80</f>
+        <f>SUM(G68:G148)/80</f>
         <v>1.1391493055555552E-2</v>
       </c>
       <c r="F166" s="83">
-        <f>SUM(G143,G140,G139,G132,G131,G123,G122,G114,G113,G105,G104,G97,G96,G89,G88,G81,G80,G74)/17</f>
+        <f>SUM(G142,G140,G139,G132,G131,G123,G122,G114,G113,G105,G104,G97,G96,G89,G88,G81,G80,G74)/17</f>
         <v>1.16489651416122E-2</v>
       </c>
       <c r="G166" s="83">
-        <f>SUM(G149,G148,G147,G146,G145,G142,G138,G137,G136,G130,G129,G128,G127,G121,G120,G119,G118,G112,G111,G110,G109,G103,G102,G101,G95,G94,G93,G87,G86,G85,G79,G78,G77,G73,G72,G71)/36</f>
+        <f>SUM(G148,G147,G146,G145,G144,G141,G138,G137,G136,G130,G129,G128,G127,G121,G120,G119,G118,G112,G111,G110,G109,G103,G102,G101,G95,G94,G93,G87,G86,G85,G79,G78,G77,G73,G72,G71)/36</f>
         <v>1.3666730967078194E-2</v>
       </c>
       <c r="H166" s="83">
-        <f>SUM(G144,G135,G134,G133,G126,G124,G125,G117,G116,G115,G108,G107,G106,G100,G99,G98,G92,G91,G90,G84,G82,G83,G76,G75,G70,G69,G68)/27</f>
+        <f>SUM(G143,G135,G134,G133,G126,G124,G125,G117,G116,G115,G108,G107,G106,G100,G99,G98,G92,G91,G90,G84,G82,G83,G76,G75,G70,G69,G68)/27</f>
         <v>8.1957304526748959E-3</v>
       </c>
       <c r="I166" s="83">
@@ -41841,7 +42138,7 @@
         <v>1.1170475520455097E-2</v>
       </c>
       <c r="K166" s="39"/>
-      <c r="L166" s="109" t="e">
+      <c r="L166" s="112" t="e">
         <f>SUM(I186-I183)/I186*100</f>
         <v>#DIV/0!</v>
       </c>
@@ -42176,11 +42473,11 @@
       </c>
       <c r="J178" s="101"/>
       <c r="K178" s="101"/>
-      <c r="L178" s="110">
+      <c r="L178" s="113">
         <f>SUM(6.25-15.35)/6.25*100</f>
         <v>-145.6</v>
       </c>
-      <c r="M178" s="139">
+      <c r="M178" s="135">
         <f>SUM(G183-I183)/G183*100</f>
         <v>-7.8050429525930678</v>
       </c>
@@ -42212,11 +42509,11 @@
       </c>
       <c r="J179" s="101"/>
       <c r="K179" s="101"/>
-      <c r="L179" s="110">
+      <c r="L179" s="113">
         <f>SUM(13.13-8.18)/13.13*100</f>
         <v>37.699923838537707</v>
       </c>
-      <c r="M179" s="138">
+      <c r="M179" s="134">
         <f>SUM(G184-I184)/G184*100</f>
         <v>-268.56633053069834</v>
       </c>
@@ -42246,11 +42543,11 @@
       </c>
       <c r="J180" s="101"/>
       <c r="K180" s="101"/>
-      <c r="L180" s="110">
+      <c r="L180" s="113">
         <f>SUM(16.11-14.18)/16.11*100</f>
         <v>11.980136561142146</v>
       </c>
-      <c r="M180" s="138">
+      <c r="M180" s="134">
         <f>SUM(G185-I185)/G185*100</f>
         <v>-224.24780284205204</v>
       </c>
@@ -42268,16 +42565,16 @@
       <c r="L181" s="102"/>
     </row>
     <row r="182" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C182" s="112" t="s">
+      <c r="C182" s="115" t="s">
         <v>68</v>
       </c>
-      <c r="D182" s="108" t="s">
+      <c r="D182" s="111" t="s">
         <v>373</v>
       </c>
-      <c r="E182" s="113" t="s">
+      <c r="E182" s="116" t="s">
         <v>370</v>
       </c>
-      <c r="F182" s="114" t="s">
+      <c r="F182" s="117" t="s">
         <v>380</v>
       </c>
       <c r="G182" s="80" t="s">
@@ -42286,66 +42583,66 @@
       <c r="H182" s="84" t="s">
         <v>377</v>
       </c>
-      <c r="I182" s="108" t="s">
+      <c r="I182" s="111" t="s">
         <v>375</v>
       </c>
-      <c r="J182" s="115" t="s">
+      <c r="J182" s="118" t="s">
         <v>377</v>
       </c>
-      <c r="K182" s="116" t="s">
+      <c r="K182" s="119" t="s">
         <v>376</v>
       </c>
-      <c r="L182" s="108" t="s">
+      <c r="L182" s="111" t="s">
         <v>924</v>
       </c>
-      <c r="M182" s="108" t="s">
+      <c r="M182" s="111" t="s">
         <v>926</v>
       </c>
-      <c r="N182" s="116" t="s">
+      <c r="N182" s="119" t="s">
         <v>925</v>
       </c>
     </row>
     <row r="183" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C183" s="117" t="s">
+      <c r="C183" s="120" t="s">
         <v>55</v>
       </c>
-      <c r="D183" s="118">
+      <c r="D183" s="121">
         <v>9</v>
       </c>
-      <c r="E183" s="118">
+      <c r="E183" s="121">
         <v>9</v>
       </c>
-      <c r="F183" s="121">
+      <c r="F183" s="124">
         <f>SUM(E183/D183)</f>
         <v>1</v>
       </c>
-      <c r="G183" s="126">
+      <c r="G183" s="130">
         <f>SUM(I74,I81,I89,I97,I105,I114,I123,I132,I140)/9</f>
         <v>22350.222222222223</v>
       </c>
-      <c r="H183" s="129">
+      <c r="H183" s="133">
         <f>_xlfn.STDEV.P(I74,I81,I89,I97,I105,I114,I123,I132,I140)</f>
         <v>8795.2952041642729</v>
       </c>
-      <c r="I183" s="123">
+      <c r="I183" s="127">
         <f>SUM(AC68,AC77,AC86,AC95,AC104,AC113,AC122,AC131,AC140)/9</f>
         <v>24094.666666666668</v>
       </c>
-      <c r="J183" s="123">
+      <c r="J183" s="127">
         <f>_xlfn.STDEV.P(AC68,AC77,AC86,AC95,AC104,AC113,AC122,AC131,AC140)</f>
         <v>6418.5518269743334</v>
       </c>
-      <c r="K183" s="111">
+      <c r="K183" s="114">
         <v>-7.8100000000000003E-2</v>
       </c>
       <c r="L183" s="94">
         <v>0.2673611111111111</v>
       </c>
-      <c r="M183" s="125">
+      <c r="M183" s="129">
         <f>SUM(AB68,AB77,AB86,AB95,AB104,AB113,AB122,AB131,AB140,AB140)/9</f>
         <v>1.0816615226337447E-2</v>
       </c>
-      <c r="N183" s="111">
+      <c r="N183" s="114">
         <v>1.456</v>
       </c>
     </row>
@@ -42353,28 +42650,28 @@
       <c r="C184" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D184" s="119">
+      <c r="D184" s="122">
         <v>9</v>
       </c>
-      <c r="E184" s="119">
+      <c r="E184" s="122">
         <v>9</v>
       </c>
-      <c r="F184" s="122">
+      <c r="F184" s="125">
         <v>1</v>
       </c>
-      <c r="G184" s="126">
+      <c r="G184" s="130">
         <f>SUM(I72,I78,I86,I94,I102,I119,I110,I128,I137)/9</f>
         <v>4109.8888888888887</v>
       </c>
-      <c r="H184" s="129">
+      <c r="H184" s="133">
         <f>_xlfn.STDEV.P(I72,I78,I86,I94,I102,I110,I119,I128,I137)</f>
         <v>913.9482655483107</v>
       </c>
-      <c r="I184" s="127">
+      <c r="I184" s="131">
         <f>SUM(H72,H78,H86,H94,H102,H110,H119,H128,H137)/9</f>
         <v>15147.666666666666</v>
       </c>
-      <c r="J184" s="127">
+      <c r="J184" s="131">
         <f>_xlfn.STDEV.P(H72,H78,H86,H94,H102,H110,H119,H128,H137)</f>
         <v>2253.2477301294089</v>
       </c>
@@ -42384,7 +42681,7 @@
       <c r="L184" s="95">
         <v>0.55069444444444449</v>
       </c>
-      <c r="M184" s="128">
+      <c r="M184" s="132">
         <f>SUM(G137,G128,G119,G110,G102,G94,G86,G78,G72)/9</f>
         <v>5.7600308641975314E-3</v>
       </c>
@@ -42396,38 +42693,38 @@
       <c r="C185" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="D185" s="120">
+      <c r="D185" s="123">
         <v>9</v>
       </c>
-      <c r="E185" s="120">
+      <c r="E185" s="123">
         <v>9</v>
       </c>
-      <c r="F185" s="122">
+      <c r="F185" s="125">
         <v>1</v>
       </c>
-      <c r="G185" s="126">
+      <c r="G185" s="130">
         <f>SUM(I70,I76,I84,I92,I100,I108,I117,I126,I135)/9</f>
         <v>10329</v>
       </c>
-      <c r="H185" s="129">
+      <c r="H185" s="133">
         <f>_xlfn.STDEV.P(I70,I76,I84,I92,I100,I108,I117,I126,I135)</f>
         <v>2050.8928678884122</v>
       </c>
-      <c r="I185" s="124">
+      <c r="I185" s="128">
         <f>SUM(H70,H76,H84,H92,H100,H108,H117,H126,H135)/9</f>
         <v>33491.555555555555</v>
       </c>
-      <c r="J185" s="124">
+      <c r="J185" s="128">
         <f>_xlfn.STDEV.P(H70,H76,H84,H92,H100,H108,H117,H126,H135)</f>
         <v>2458.4264213386177</v>
       </c>
-      <c r="K185" s="70">
+      <c r="K185" s="68">
         <v>-2.2423999999999999</v>
       </c>
       <c r="L185" s="95">
         <v>0.6743055555555556</v>
       </c>
-      <c r="M185" s="128">
+      <c r="M185" s="132">
         <f>SUM(G70,G76,G84,G92,G100,G108,G117,G126,G135)/9</f>
         <v>9.9279835390946505E-3</v>
       </c>
@@ -42436,24 +42733,168 @@
       </c>
     </row>
     <row r="186" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C186" s="130"/>
-      <c r="D186" s="131"/>
-      <c r="E186" s="131"/>
-      <c r="F186" s="132"/>
-      <c r="G186" s="91"/>
-      <c r="H186" s="91"/>
-      <c r="I186" s="133"/>
-      <c r="J186" s="134"/>
-      <c r="K186" s="132"/>
-      <c r="L186" s="135"/>
-      <c r="M186" s="136"/>
-      <c r="N186" s="137"/>
+      <c r="C186" s="108"/>
+      <c r="D186" s="136"/>
+      <c r="E186" s="136"/>
+      <c r="F186" s="110"/>
+      <c r="G186" s="109"/>
+      <c r="H186" s="109"/>
+      <c r="I186" s="137"/>
+      <c r="J186" s="137"/>
+      <c r="K186" s="110"/>
+      <c r="L186" s="138"/>
+      <c r="M186" s="139"/>
+      <c r="N186" s="110"/>
+    </row>
+    <row r="187" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C187" s="115" t="s">
+        <v>68</v>
+      </c>
+      <c r="D187" s="111" t="s">
+        <v>373</v>
+      </c>
+      <c r="E187" s="116"/>
+      <c r="F187" s="117" t="s">
+        <v>380</v>
+      </c>
+      <c r="G187" s="80" t="s">
+        <v>374</v>
+      </c>
+      <c r="H187" s="84" t="s">
+        <v>377</v>
+      </c>
+      <c r="I187" s="111" t="s">
+        <v>375</v>
+      </c>
+      <c r="J187" s="118" t="s">
+        <v>377</v>
+      </c>
+      <c r="K187" s="119" t="s">
+        <v>376</v>
+      </c>
+      <c r="L187" s="111" t="s">
+        <v>924</v>
+      </c>
+      <c r="M187" s="111" t="s">
+        <v>926</v>
+      </c>
+      <c r="N187" s="119" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="188" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C188" s="120" t="s">
+        <v>55</v>
+      </c>
+      <c r="D188" s="121">
+        <v>9</v>
+      </c>
+      <c r="E188" s="121"/>
+      <c r="F188" s="124">
+        <v>1</v>
+      </c>
+      <c r="G188" s="130">
+        <v>22350.222222222223</v>
+      </c>
+      <c r="H188" s="133">
+        <v>8795.2952041642729</v>
+      </c>
+      <c r="I188" s="127">
+        <v>24094.666666666668</v>
+      </c>
+      <c r="J188" s="127">
+        <v>6418.5518269743334</v>
+      </c>
+      <c r="K188" s="114">
+        <v>-7.8100000000000003E-2</v>
+      </c>
+      <c r="L188" s="94">
+        <v>0.2673611111111111</v>
+      </c>
+      <c r="M188" s="129">
+        <v>1.0816615226337447E-2</v>
+      </c>
+      <c r="N188" s="114">
+        <v>1.456</v>
+      </c>
+    </row>
+    <row r="189" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C189" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D189" s="122">
+        <v>9</v>
+      </c>
+      <c r="E189" s="122"/>
+      <c r="F189" s="125">
+        <v>1</v>
+      </c>
+      <c r="G189" s="130">
+        <v>4109.8888888888887</v>
+      </c>
+      <c r="H189" s="133">
+        <v>913.9482655483107</v>
+      </c>
+      <c r="I189" s="131">
+        <v>15147.666666666666</v>
+      </c>
+      <c r="J189" s="131">
+        <v>2253.2477301294089</v>
+      </c>
+      <c r="K189" s="68">
+        <v>-2.6856</v>
+      </c>
+      <c r="L189" s="95">
+        <v>0.55069444444444449</v>
+      </c>
+      <c r="M189" s="132">
+        <v>5.7600308641975314E-3</v>
+      </c>
+      <c r="N189" s="68">
+        <v>-0.377</v>
+      </c>
+    </row>
+    <row r="190" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C190" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="D190" s="140">
+        <v>9</v>
+      </c>
+      <c r="E190" s="140"/>
+      <c r="F190" s="126">
+        <v>1</v>
+      </c>
+      <c r="G190" s="141">
+        <v>10329</v>
+      </c>
+      <c r="H190" s="142">
+        <v>2050.8928678884122</v>
+      </c>
+      <c r="I190" s="143">
+        <v>33491.555555555555</v>
+      </c>
+      <c r="J190" s="143">
+        <v>2458.4264213386177</v>
+      </c>
+      <c r="K190" s="70">
+        <v>-2.2423999999999999</v>
+      </c>
+      <c r="L190" s="144">
+        <v>0.6743055555555556</v>
+      </c>
+      <c r="M190" s="145">
+        <v>9.9279835390946505E-3</v>
+      </c>
+      <c r="N190" s="70">
+        <v>-0.1198</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A67:T140" xr:uid="{9B513DDC-6C9C-43F7-A6B4-DFFF987F6CC7}">
+  <autoFilter ref="A67:T148" xr:uid="{9B513DDC-6C9C-43F7-A6B4-DFFF987F6CC7}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Iron"/>
+        <filter val="POSH-core"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -42602,21 +43043,21 @@
     <hyperlink ref="C139" r:id="rId142" display="html/replays/POSH-CORE/00367-POSH_CIME.REP" xr:uid="{D81AA046-FFEF-46D4-AEE2-2F91CDA1FB32}"/>
     <hyperlink ref="B140" r:id="rId143" display="html/replays/ZZZKBOT/00368-ZZZK_POSH.REP" xr:uid="{4F509912-7D87-42E3-BDEF-8F3583376804}"/>
     <hyperlink ref="C140" r:id="rId144" display="html/replays/POSH-CORE/00368-POSH_ZZZK.REP" xr:uid="{0C429ECD-71AF-43E9-87E8-0AE4E6F07641}"/>
-    <hyperlink ref="B142" r:id="rId145" display="html/replays/POSH-CORE/00006-POSH_ORIT.REP" xr:uid="{FFAAB4EC-CA95-40B4-9E97-51088B7A761C}"/>
-    <hyperlink ref="C142" r:id="rId146" display="html/replays/ORITAKA/00006-ORIT_POSH.REP" xr:uid="{B8E893ED-14F2-4CC1-870B-C283E44C230A}"/>
-    <hyperlink ref="B143" r:id="rId147" display="html/replays/POSH-CORE/00007-POSH_CIME.REP" xr:uid="{7F98EA1F-B2CC-410E-921A-D7D3C6EA392C}"/>
-    <hyperlink ref="C143" r:id="rId148" display="html/replays/CIMEX/00007-CIME_POSH.REP" xr:uid="{2C29D367-8947-44C6-8E94-C547E0F670A7}"/>
-    <hyperlink ref="B144" r:id="rId149" display="html/replays/POSH-CORE/00046-POSH_MEGA.REP" xr:uid="{A21A28A3-3BE7-46D9-8EF2-58D069D868B8}"/>
-    <hyperlink ref="B145" r:id="rId150" display="html/replays/POSH-CORE/00051-POSH_ORIT.REP" xr:uid="{03E6A83D-D256-4908-B233-B4D01409897D}"/>
-    <hyperlink ref="C145" r:id="rId151" display="html/replays/ORITAKA/00051-ORIT_POSH.REP" xr:uid="{11F3F0E4-CADB-4685-A978-13D276850621}"/>
-    <hyperlink ref="B146" r:id="rId152" display="html/replays/POSH-CORE/00096-POSH_ORIT.REP" xr:uid="{24D64762-3114-47F8-BDF4-2AF3DD37F61C}"/>
-    <hyperlink ref="C146" r:id="rId153" display="html/replays/ORITAKA/00096-ORIT_POSH.REP" xr:uid="{ACD1154D-68F7-4191-BDBA-235AC42D7FF7}"/>
-    <hyperlink ref="B147" r:id="rId154" display="html/replays/POSH-CORE/00141-POSH_ORIT.REP" xr:uid="{A62C1B32-D74C-4AC1-A8A8-B02357B49B06}"/>
-    <hyperlink ref="C147" r:id="rId155" display="html/replays/ORITAKA/00141-ORIT_POSH.REP" xr:uid="{19DDB3E2-4B88-402A-9BB9-CD8612DEE7C4}"/>
-    <hyperlink ref="B148" r:id="rId156" display="html/replays/POSH-CORE/00186-POSH_ORIT.REP" xr:uid="{10023D3C-B8ED-4C54-95CD-2864825F9373}"/>
-    <hyperlink ref="C148" r:id="rId157" display="html/replays/ORITAKA/00186-ORIT_POSH.REP" xr:uid="{8057A31E-C568-4F96-9E7F-BFF8ECFA4EB1}"/>
-    <hyperlink ref="B149" r:id="rId158" display="html/replays/POSH-CORE/00366-POSH_ORIT.REP" xr:uid="{C813A1B3-C800-4C0D-ACDC-3BF5AC107EB3}"/>
-    <hyperlink ref="C149" r:id="rId159" display="html/replays/ORITAKA/00366-ORIT_POSH.REP" xr:uid="{FB2D833D-122D-4883-87E2-8574026A3417}"/>
+    <hyperlink ref="B141" r:id="rId145" display="html/replays/POSH-CORE/00006-POSH_ORIT.REP" xr:uid="{FFAAB4EC-CA95-40B4-9E97-51088B7A761C}"/>
+    <hyperlink ref="C141" r:id="rId146" display="html/replays/ORITAKA/00006-ORIT_POSH.REP" xr:uid="{B8E893ED-14F2-4CC1-870B-C283E44C230A}"/>
+    <hyperlink ref="B142" r:id="rId147" display="html/replays/POSH-CORE/00007-POSH_CIME.REP" xr:uid="{7F98EA1F-B2CC-410E-921A-D7D3C6EA392C}"/>
+    <hyperlink ref="C142" r:id="rId148" display="html/replays/CIMEX/00007-CIME_POSH.REP" xr:uid="{2C29D367-8947-44C6-8E94-C547E0F670A7}"/>
+    <hyperlink ref="B143" r:id="rId149" display="html/replays/POSH-CORE/00046-POSH_MEGA.REP" xr:uid="{A21A28A3-3BE7-46D9-8EF2-58D069D868B8}"/>
+    <hyperlink ref="B144" r:id="rId150" display="html/replays/POSH-CORE/00051-POSH_ORIT.REP" xr:uid="{03E6A83D-D256-4908-B233-B4D01409897D}"/>
+    <hyperlink ref="C144" r:id="rId151" display="html/replays/ORITAKA/00051-ORIT_POSH.REP" xr:uid="{11F3F0E4-CADB-4685-A978-13D276850621}"/>
+    <hyperlink ref="B145" r:id="rId152" display="html/replays/POSH-CORE/00096-POSH_ORIT.REP" xr:uid="{24D64762-3114-47F8-BDF4-2AF3DD37F61C}"/>
+    <hyperlink ref="C145" r:id="rId153" display="html/replays/ORITAKA/00096-ORIT_POSH.REP" xr:uid="{ACD1154D-68F7-4191-BDBA-235AC42D7FF7}"/>
+    <hyperlink ref="B146" r:id="rId154" display="html/replays/POSH-CORE/00141-POSH_ORIT.REP" xr:uid="{A62C1B32-D74C-4AC1-A8A8-B02357B49B06}"/>
+    <hyperlink ref="C146" r:id="rId155" display="html/replays/ORITAKA/00141-ORIT_POSH.REP" xr:uid="{19DDB3E2-4B88-402A-9BB9-CD8612DEE7C4}"/>
+    <hyperlink ref="B147" r:id="rId156" display="html/replays/POSH-CORE/00186-POSH_ORIT.REP" xr:uid="{10023D3C-B8ED-4C54-95CD-2864825F9373}"/>
+    <hyperlink ref="C147" r:id="rId157" display="html/replays/ORITAKA/00186-ORIT_POSH.REP" xr:uid="{8057A31E-C568-4F96-9E7F-BFF8ECFA4EB1}"/>
+    <hyperlink ref="B148" r:id="rId158" display="html/replays/POSH-CORE/00366-POSH_ORIT.REP" xr:uid="{C813A1B3-C800-4C0D-ACDC-3BF5AC107EB3}"/>
+    <hyperlink ref="C148" r:id="rId159" display="html/replays/ORITAKA/00366-ORIT_POSH.REP" xr:uid="{FB2D833D-122D-4883-87E2-8574026A3417}"/>
     <hyperlink ref="X148" r:id="rId160" display="html/replays/CIMEX/00404-CIME_ZZZK.REP" xr:uid="{4A702588-E210-470F-AFC1-839DC51D005F}"/>
     <hyperlink ref="W148" r:id="rId161" display="html/replays/ZZZKBOT/00404-ZZZK_CIME.REP" xr:uid="{DA06ADC2-2FC5-461F-A32A-EAEBB10ED194}"/>
     <hyperlink ref="X147" r:id="rId162" display="html/replays/ORITAKA/00403-ORIT_ZZZK.REP" xr:uid="{D8A0DD24-FB71-4E6F-AE7C-B10CE6BD739B}"/>

</xml_diff>